<commit_message>
profile page test scripts
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oversight Training\TrainingProjectOversight\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053AEFF7-DBC6-400F-92F2-2B1FFE4C6653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC9DCEF-7ECA-455A-B456-0948023D4EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="3360" windowWidth="22284" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{F05D039A-02BA-444C-94CA-C8E6424376EB}"/>
+    <workbookView xWindow="372" yWindow="3360" windowWidth="22284" windowHeight="8880" firstSheet="1" activeTab="3" xr2:uid="{F05D039A-02BA-444C-94CA-C8E6424376EB}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="register" sheetId="2" r:id="rId2"/>
-    <sheet name="billingSpace" sheetId="4" r:id="rId3"/>
-    <sheet name="subSpace" sheetId="5" r:id="rId4"/>
-    <sheet name="controller" sheetId="6" r:id="rId5"/>
-    <sheet name="device" sheetId="7" r:id="rId6"/>
-    <sheet name="WrongCredentials" sheetId="8" r:id="rId7"/>
-    <sheet name="billingAccount" sheetId="3" r:id="rId8"/>
+    <sheet name="password" sheetId="9" r:id="rId2"/>
+    <sheet name="email" sheetId="10" r:id="rId3"/>
+    <sheet name="existEmail" sheetId="11" r:id="rId4"/>
+    <sheet name="register" sheetId="2" r:id="rId5"/>
+    <sheet name="billingSpace" sheetId="4" r:id="rId6"/>
+    <sheet name="subSpace" sheetId="5" r:id="rId7"/>
+    <sheet name="controller" sheetId="6" r:id="rId8"/>
+    <sheet name="device" sheetId="7" r:id="rId9"/>
+    <sheet name="WrongCredentials" sheetId="8" r:id="rId10"/>
+    <sheet name="billingAccount" sheetId="3" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -76,24 +79,6 @@
     <t>confirmPassword</t>
   </si>
   <si>
-    <t>Pawani</t>
-  </si>
-  <si>
-    <t>Chethana</t>
-  </si>
-  <si>
-    <t>Pawani_Che</t>
-  </si>
-  <si>
-    <t>986578745v</t>
-  </si>
-  <si>
-    <t>pawani@yopmail.com</t>
-  </si>
-  <si>
-    <t>Pawani12#</t>
-  </si>
-  <si>
     <t>billingLabel</t>
   </si>
   <si>
@@ -157,7 +142,34 @@
     <t>Saduni1997#</t>
   </si>
   <si>
-    <t>0786745678</t>
+    <t>Dasuni</t>
+  </si>
+  <si>
+    <t>Niwanthika</t>
+  </si>
+  <si>
+    <t>Dasuni_new</t>
+  </si>
+  <si>
+    <t>986578790v</t>
+  </si>
+  <si>
+    <t>0786295678</t>
+  </si>
+  <si>
+    <t>dasuni@yopmail.com</t>
+  </si>
+  <si>
+    <t>Dasuni12#</t>
+  </si>
+  <si>
+    <t>sanduni1998@yopmail.com</t>
+  </si>
+  <si>
+    <t>existEmail</t>
+  </si>
+  <si>
+    <t>oversight_user@syntaxgenie.com</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -236,6 +248,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -554,7 +567,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,12 +597,179 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982BE54E-9DCF-4DA3-985F-07BFBC415DC0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D654056B-BBF9-4707-B464-837357ACA015}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4">
+        <v>98765476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2474E8-5639-49DE-88D8-C927F8195A4E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5E8920-072B-4DEA-8C55-BFFA1FC88FF2}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E3A6AB04-662F-4ACF-ACD7-F0C70086FEED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F932AC-4BAD-4FED-8D77-6081DD12AEB0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{802EAC5C-0755-4CC5-9BB1-D7578E607B43}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D612D7-DC16-47A1-81F5-3E817A00DC87}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,28 +812,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB27384D-63C1-4024-AC3C-8AAEAD2B6842}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -680,20 +860,20 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537AD7EA-7DC9-4D2D-863C-13C358E9FD38}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -708,20 +888,20 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71320601-33E2-42C9-932A-C31C77A1D4B6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -737,18 +917,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421D8DFB-4B14-4218-96E9-935A60D6319C}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -773,28 +953,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4">
         <v>30</v>
@@ -804,74 +984,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982BE54E-9DCF-4DA3-985F-07BFBC415DC0}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D654056B-BBF9-4707-B464-837357ACA015}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4">
-        <v>98765476</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>